<commit_message>
Entry added for 10/10/2017
</commit_message>
<xml_diff>
--- a/DailyTicketReport.xlsx
+++ b/DailyTicketReport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="146">
   <si>
     <t>Benson Fabonan</t>
   </si>
@@ -331,15 +331,7 @@
     <t>Inova : Please retrieve and process TEST files (Inova sFTP test)</t>
   </si>
   <si>
-    <t>- No Issue
-- The key provided is the same with what currently is being used. Requested for a screenshot of error.</t>
-  </si>
-  <si>
     <t>Bechtel  : Unable to Block certain type of employees</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Logged a request to block the user in UAT. See IXS-10850494.</t>
   </si>
   <si>
     <t>Genesis : Data file coming back to us</t>
@@ -370,15 +362,7 @@
     <t>Inova :  Please run Offcycle Import in Prod</t>
   </si>
   <si>
-    <t>- No Issue
-- Offcycle run completed successfully for 9/6 files.</t>
-  </si>
-  <si>
     <t>Inova : Export Duplicate records being sent</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Informed AM that we forgot to run the Post Action script manually.</t>
   </si>
   <si>
     <t xml:space="preserve">- No Issue
@@ -400,18 +384,10 @@
     <t xml:space="preserve">Kellogg : User not found on Daily Ticket Report </t>
   </si>
   <si>
-    <t>- No Issue
-- The user was rejected as the JobTitle exceeded the 50 characters limit.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CofPA : Request to Toggle on W-2 Election</t>
   </si>
   <si>
     <t>Hurley Medical  :  FYI - Daily file processing will be suspended</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Acknowledged the information provided about the upgrade.</t>
   </si>
   <si>
     <t>Fixed</t>
@@ -441,10 +417,6 @@
   </si>
   <si>
     <t>- No Issue
-- Requested file provided.</t>
-  </si>
-  <si>
-    <t>- No Issue
 - Client wants to be done on UAT</t>
   </si>
   <si>
@@ -484,13 +456,6 @@
 - Informed AM that Jeric only said that the user was already exported</t>
   </si>
   <si>
-    <t>HCA : Changes in the import xriteria for Marital Status</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Rolled back changes</t>
-  </si>
-  <si>
     <t>PGE : Duplicate Enwisen files on 8/8/17 file</t>
   </si>
   <si>
@@ -498,14 +463,36 @@
 - The issue was replicated in UAT and the export flag of user did change from 2 to 0 thus causing duplicate export. DBA team said they didn't find any script that updates the flag. Informed AM to contact dev team to check.</t>
   </si>
   <si>
-    <t>Aetna : Changes to SSIS Import Notifications</t>
-  </si>
-  <si>
     <t>- No Issue
 - Responded to AM's additional inquiries.</t>
   </si>
   <si>
-    <t>Nissan CM Export outbound file request in Prod</t>
+    <t>- No Issue
+- Re-deployed changed to prod</t>
+  </si>
+  <si>
+    <t>HCA : Changes in the import criteria for Marital Status</t>
+  </si>
+  <si>
+    <t>MoheganSun : Missing an Employee</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Error log was set also to 5 days. Please let me know if the client wants to change its value so that we may check longer days of error logs in the future.</t>
+  </si>
+  <si>
+    <t>Kellogg  :  A. Schumacher not in CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- No Issue
+- The 5 names below were the only user with lastname 'Schumacher' found on </t>
+  </si>
+  <si>
+    <t>PGE :  Unable to update Date of Birth for New Hire, Alejandro Ruiz, 08184</t>
+  </si>
+  <si>
+    <t>- No Issue
+- As per checking, I found that the value for user 08322 on DateofBirth field is '11/25/2022 12:00:00 AM'. No error and warning found in the latest file.</t>
   </si>
 </sst>
 </file>
@@ -618,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -668,6 +655,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -983,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,221 +1008,225 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>10975120</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>10238881</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>10238881</v>
+        <v>10951207</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>10951207</v>
+        <v>10959479</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>10959326</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>10959479</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>126</v>
-      </c>
       <c r="D6" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>10959326</v>
+        <v>10958526</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>10958526</v>
+        <v>10794689</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>10794689</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="16"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>10971301</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10912397</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>10978794</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>10916620</v>
+        <v>10978677</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>10645887</v>
+        <v>10916620</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>10856950</v>
+        <v>10645887</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>10710067</v>
+        <v>10856950</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>10888165</v>
+        <v>10710067</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>10857470</v>
+        <v>10888165</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>104</v>
@@ -1244,12 +1238,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>10710067</v>
+        <v>10857470</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
@@ -1258,53 +1252,61 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>10766794</v>
+        <v>10710067</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>10733303</v>
+        <v>10766794</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>10733303</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>10733303</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
@@ -1313,262 +1315,254 @@
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="16"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C29" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>10652232</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>10781938</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>10952117</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>10866854</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>10901853</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>10941499</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>10956013</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="18"/>
+    </row>
+    <row r="37" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>10857617</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>10964763</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>10951207</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>10956802</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>10956804</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>10956013</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>10760153</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>10952117</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>10941499</v>
-      </c>
       <c r="B37" s="2" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>10741424</v>
+        <v>10964763</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>10652232</v>
+        <v>10951207</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>10901853</v>
+        <v>10956802</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>10866854</v>
+        <v>10956804</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>10781938</v>
+        <v>10760153</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>10652232</v>
+        <v>10741424</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>10732806</v>
+        <v>10652232</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>10719864</v>
+        <v>10732806</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>10719864</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added entry for 10/24
</commit_message>
<xml_diff>
--- a/DailyTicketReport.xlsx
+++ b/DailyTicketReport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="149">
   <si>
     <t>Benson Fabonan</t>
   </si>
@@ -277,26 +277,12 @@
   </si>
   <si>
     <t>TriHealth : JobDesc Import Success Notice</t>
-  </si>
-  <si>
-    <t>CofPA : Employees not being assigned basic access</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- No Issue
-- We are not the one setting up Bulk Group Assignment. As per checking, BGA runs daily at 2:45AM. No failure email notification received regarding BGA. </t>
   </si>
   <si>
     <t>- No Issue
 - Sent details explanation on the newhire and census jobs</t>
   </si>
   <si>
-    <t>PGE : (Portland General Electric) TS Upgrade: SSIS Analysis</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Responded to inquiry regarding job schedules.</t>
-  </si>
-  <si>
     <t>SanfordHealth  : Request to modify Orientation fields within Manage New Hire</t>
   </si>
   <si>
@@ -311,9 +297,6 @@
     <t>CofPA :I-9 Verifiers not transitioning to the Other Tab form</t>
   </si>
   <si>
-    <t>Genesis : Data file coming back to us</t>
-  </si>
-  <si>
     <t>- No Issue
 - Startdate was being used only by Completed NewHires Forms export to determine that the user could be exported only after he/she completed the forms not later than 12 days of his/her startdate</t>
   </si>
@@ -325,17 +308,6 @@
 - User's data will be wiped out once 'Custom8' has a value of 'Yes'.This user was imported 2016-07-11. Archived files were not available or deleted later than 20170101 for SUMMA.</t>
   </si>
   <si>
-    <t>RockwellAutomation : Updating Custom9 character limit in Kenexa new hire import</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Code has been sent for deployment on UAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- No Issue
-- Advise what is the field and table used for "County" for client Genesis? </t>
-  </si>
-  <si>
     <t>Trihealth : query on directory user profile in Case Management</t>
   </si>
   <si>
@@ -387,10 +359,6 @@
   </si>
   <si>
     <t>- No Issue
-- The issue was replicated in UAT and the export flag of user did change from 2 to 0 thus causing duplicate export. DBA team said they didn't find any script that updates the flag. Informed AM to contact dev team to check.</t>
-  </si>
-  <si>
-    <t>- No Issue
 - Responded to AM's additional inquiries.</t>
   </si>
   <si>
@@ -401,9 +369,6 @@
 - Error log was set also to 5 days. Please let me know if the client wants to change its value so that we may check longer days of error logs in the future.</t>
   </si>
   <si>
-    <t>Kellogg  :  A. Schumacher not in CM</t>
-  </si>
-  <si>
     <t>PGE :  Unable to update Date of Birth for New Hire, Alejandro Ruiz, 08184</t>
   </si>
   <si>
@@ -421,33 +386,11 @@
     <t>Bechtel : Data not being sent in Data dump files</t>
   </si>
   <si>
-    <t>- No Issue
-- Ticket codes is not eligible for export.</t>
-  </si>
-  <si>
     <t>HCA : UAT - new hire import</t>
   </si>
   <si>
     <t>- No Issue
 - UAT job ran</t>
-  </si>
-  <si>
-    <t>Bechtel : PIck up separate file feedimport</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Prod census import job ran</t>
-  </si>
-  <si>
-    <t>Inova : Manual load of onboarding file needed</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Run an offcycle import the file is located in Production/Inbound inova_newhire_20171011.txt.pgp</t>
-  </si>
-  <si>
-    <t>- No Issue
-- I can't find this 'Sridevi Yerukalapudi' user in the latest file. kellogg_census_20171010.txt. However, I see ashley schumacher now. Userid is 204029.</t>
   </si>
   <si>
     <t>ConAgra : Need notification changed from HRMS to HRDataandAnalysis@conagra.com</t>
@@ -468,10 +411,6 @@
     <t>Troutman Sanders : New hire import</t>
   </si>
   <si>
-    <t>- No Issue
-- There were no files uploaded for 10/11/2017 that is why there were no results.</t>
-  </si>
-  <si>
     <t>BectonDickinson :  full time associate does not have access to HR One</t>
   </si>
   <si>
@@ -482,9 +421,6 @@
 - Done as requested. File attached to ticket.</t>
   </si>
   <si>
-    <t>SpeedwayMarathon : Export files request</t>
-  </si>
-  <si>
     <t>- No Issue
 - Done as requested</t>
   </si>
@@ -492,36 +428,7 @@
     <t xml:space="preserve"> NavyFederal  : Please reflag users 56502 and 56503</t>
   </si>
   <si>
-    <t>PNC : Update to communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- No Issue
-- Request has been logged to deploy changes in PROD.
-See IXS-10983829.
-</t>
-  </si>
-  <si>
-    <t>URBN : EEPDML files request</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Requested files provided.</t>
-  </si>
-  <si>
-    <t>GDIT ~ HR404E PDF update Orientation tour v.19 and CSR tour v.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- No Issue
-- Request has been logged to deploy changes in PROD.
-See IXS-10984994.
-</t>
-  </si>
-  <si>
     <t>EY : Off cycle UAT -Import</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Run done, users does not have enwuserid wich is a required field.</t>
   </si>
   <si>
     <t>- No Issue
@@ -542,10 +449,6 @@
     <t>This is for MCC changes for Hersheys</t>
   </si>
   <si>
-    <t>- No Issue
-- This is for MCC changes for Hersheys</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CofPA : I9 approver failed to populate on Tracker I9 Tab</t>
   </si>
   <si>
@@ -564,7 +467,42 @@
     <t>EDMC :  KB Upgrade: SSIS Analysis</t>
   </si>
   <si>
-    <t>PNC Bank : New Hire PDF and Flat File Export Failure Notice on hrsdpp02-l</t>
+    <t>Sena :  Adding documents to onboarding tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- No Issue
+- As per checking, this fields were not included to current export flat file and PDF's. May I know if this is a new PDF export implementation or an update to existing export flat file or PDF? If this is new PDF export implementation I think this belongs to ICS team. Kindly confirm with client. </t>
+  </si>
+  <si>
+    <t>EY : Job Description Import Special Run</t>
+  </si>
+  <si>
+    <t>EY : Requesting Import Specs</t>
+  </si>
+  <si>
+    <t>- No Issue
+- EY mapping attached to ticket</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Confirmed that the fix worked.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- The date diff makes the ticked not eligible for export, but upon further inspection the 5 give ticket codes were already exported which matches the last edit date.</t>
+  </si>
+  <si>
+    <t>NavyFederal : Reflag user 51196R01</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Files were downloaded from August 1-9</t>
+  </si>
+  <si>
+    <t>IronMountain : export files and check path existence request</t>
+  </si>
+  <si>
+    <t>Nissan : CM Export outbound file request in UAT</t>
   </si>
 </sst>
 </file>
@@ -712,10 +650,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1032,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,232 +1005,228 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <v>10998002</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>164</v>
+        <v>10863530</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>10968452</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>10863530</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>10988718</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>10986080</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>10988718</v>
+        <v>10981491</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>10986080</v>
+        <v>10982874</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>10981491</v>
+        <v>10981895</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>10982874</v>
+        <v>10968040</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>10981895</v>
+        <v>10951207</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10968040</v>
+        <v>10959479</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10951207</v>
+        <v>10959326</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>10959479</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>10959326</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="14"/>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>11002328</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>11002597</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
+        <v>10919383</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>10710067</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>10988718</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>143</v>
+      <c r="D20" s="9" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -1300,13 +1234,13 @@
         <v>10986362</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1314,13 +1248,13 @@
         <v>10982995</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1328,439 +1262,351 @@
         <v>10984740</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>10986074</v>
+        <v>10985054</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>10985054</v>
+        <v>10982909</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>10982909</v>
+        <v>10912397</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10982663</v>
+        <v>10978677</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>10912397</v>
+        <v>10916620</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>10978794</v>
+        <v>10645887</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>10978677</v>
+        <v>10857470</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>10916620</v>
+        <v>10710067</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>10733303</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>11010570</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>11011839</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>10981895</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>11009444</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>10857617</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>10645887</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>10856950</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="9" t="s">
+      <c r="C41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>10956804</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>10956802</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>10888165</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>10857470</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>10710067</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>10733303</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>10733303</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="18">
-        <v>10956804</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>10956802</v>
+        <v>10982995</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>162</v>
+      <c r="D44" s="9" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>10982995</v>
+        <v>10978777</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>10951207</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>10983470</v>
+        <v>10956804</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>10929553</v>
+        <v>10732806</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>10978777</v>
+        <v>10719864</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>10857617</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>10951207</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>10956804</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>10741424</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>10732806</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>10719864</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>90</v>
+      <c r="D49" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added entry for 11/09
</commit_message>
<xml_diff>
--- a/DailyTicketReport.xlsx
+++ b/DailyTicketReport.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="149">
-  <si>
-    <t>Benson Fabonan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="153">
   <si>
     <t>Ticket</t>
   </si>
@@ -277,10 +274,6 @@
   </si>
   <si>
     <t>TriHealth : JobDesc Import Success Notice</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Sent details explanation on the newhire and census jobs</t>
   </si>
   <si>
     <t>SanfordHealth  : Request to modify Orientation fields within Manage New Hire</t>
@@ -317,9 +310,6 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>Trihealth: Inquiry on user James Burton</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -340,19 +330,7 @@
 - Development in progress</t>
   </si>
   <si>
-    <t>- No Issue
-- Informed AM that they should provide a date range where we can look for the user in the import file</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Done as requested.</t>
-  </si>
-  <si>
     <t>GDIT : HR404E PDF update Orientation tour v.19 and CSR tour v.16</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Informed AM that Jeric only said that the user was already exported</t>
   </si>
   <si>
     <t>PGE : Duplicate Enwisen files on 8/8/17 file</t>
@@ -379,25 +357,10 @@
     <t>SENA : Suez/Sena Import/Export</t>
   </si>
   <si>
-    <t>- No Issue
-- Attached sample file.</t>
-  </si>
-  <si>
     <t>Bechtel : Data not being sent in Data dump files</t>
   </si>
   <si>
-    <t>HCA : UAT - new hire import</t>
-  </si>
-  <si>
-    <t>- No Issue
-- UAT job ran</t>
-  </si>
-  <si>
     <t>ConAgra : Need notification changed from HRMS to HRDataandAnalysis@conagra.com</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Clarified what email notif is to be updated.</t>
   </si>
   <si>
     <t>PNC : New Hire Import Success Notice on hrsdpp02-m</t>
@@ -408,17 +371,10 @@
 Screenshot shows that the file uploaded has 0KB in size.</t>
   </si>
   <si>
-    <t>Troutman Sanders : New hire import</t>
-  </si>
-  <si>
     <t>BectonDickinson :  full time associate does not have access to HR One</t>
   </si>
   <si>
     <t>JPSHealth ~ New hire file</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Done as requested. File attached to ticket.</t>
   </si>
   <si>
     <t>- No Issue
@@ -428,13 +384,6 @@
     <t xml:space="preserve"> NavyFederal  : Please reflag users 56502 and 56503</t>
   </si>
   <si>
-    <t>EY : Off cycle UAT -Import</t>
-  </si>
-  <si>
-    <t>- No Issue
-- File attached to ticket</t>
-  </si>
-  <si>
     <t>NavyFederal  : DMARC implementation requires DNS changes for all OB emails</t>
   </si>
   <si>
@@ -446,18 +395,7 @@
 - Clarified the exact request from Cherry.</t>
   </si>
   <si>
-    <t>This is for MCC changes for Hersheys</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CofPA : I9 approver failed to populate on Tracker I9 Tab</t>
-  </si>
-  <si>
-    <t>- No Issue
-- 00739169 userid was sent via newhire(as rehire data) but not included on the census file. This 00739169 userid should also be included on census file at the same day it was sent as a newhire. Census file 'positionnumber' will determine the value of the user's I9ApproverUserID and I9ApproverName on the same day only.</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Update allowed after import set to yes for role3,hiredate and startdate on UAT.</t>
   </si>
   <si>
     <t>- No Issue
@@ -499,10 +437,83 @@
 - Files were downloaded from August 1-9</t>
   </si>
   <si>
-    <t>IronMountain : export files and check path existence request</t>
-  </si>
-  <si>
-    <t>Nissan : CM Export outbound file request in UAT</t>
+    <t>- No Issue
+- Attached the screenshot showing all files from August 1-9 was downloaded and is still available for pickup</t>
+  </si>
+  <si>
+    <t>GeneralDynamics : Missing PDF for Juan Gomez Rodriguez</t>
+  </si>
+  <si>
+    <t>- No Issue
+- User W312057 PoliciesAck reflagged. User will be exported on the next automated export job run.</t>
+  </si>
+  <si>
+    <t>Bechtel : Language displayed on MyHR Services for an employee on international assignment</t>
+  </si>
+  <si>
+    <t>- No Issue
+- This is done as requested to UAT and Prod.</t>
+  </si>
+  <si>
+    <t>BannerHealth :  Letters to new hires</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inova Export File Request in UAT</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Informed ICS that files are not existing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BannerHealth  : Full Tour not available to New Hires</t>
+  </si>
+  <si>
+    <t>AIR : new hire notification not sent</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Informed AM that there is another file on the path.</t>
+  </si>
+  <si>
+    <t>Bridgestone : UAT manual run</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Done in UAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- No Issue
+- Can't find a user with I9VerifierPosNo = '50494234' in newhire. This might cause the NULL value for the user's I9ApproverUserID and I9ApproverName. </t>
+  </si>
+  <si>
+    <t>Benson Fabonan</t>
+  </si>
+  <si>
+    <t>Nissan : ICS File request</t>
+  </si>
+  <si>
+    <t>GDIT : Query on How the "Role2" field is being populated</t>
+  </si>
+  <si>
+    <t>- No Issue
+- I found sample userid with role2 = Y</t>
+  </si>
+  <si>
+    <t>Bridgestone : Load test file into UAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- No Issue
+- I tried to process the UAT file but I received an error on the email notification. Please check attached file. I will create a test environment to see were it fails on specific parts of the import process but I might take some time. Can we have smaller test user count to test it properly? </t>
+  </si>
+  <si>
+    <t>EY : Off-cycle request</t>
+  </si>
+  <si>
+    <t>Inova : Manager did not see manager separtion checklist in their offboarding</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Request logged to deploy changes in PROD. IXS-11040393</t>
   </si>
 </sst>
 </file>
@@ -653,8 +664,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,87 +997,87 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>10863530</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="16"/>
+      <c r="A3" s="10">
+        <v>11045499</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <v>10988718</v>
+        <v>10968040</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <v>10986080</v>
+        <v>11013376</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
+        <v>10981895</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>10981491</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>10982874</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1074,539 +1085,603 @@
         <v>10981895</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>10959479</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>10984740</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>10968040</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>11018684</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>10710067</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>10982909</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>10645887</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>10985054</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>10951207</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10959479</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>10959326</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C19" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>10733303</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>11013376</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>11002328</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>11002597</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>10919383</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>10710067</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="D21" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>11033219</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>10986362</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>10982995</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>10984740</v>
-      </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>10985054</v>
+        <v>10942832</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>10982909</v>
+        <v>10982995</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>10912397</v>
+        <v>11015181</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10978677</v>
+        <v>11002328</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
+        <v>11002597</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>10919383</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>10982995</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>10912397</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>10978677</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>10916620</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>10645887</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>10857470</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>10710067</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>11009444</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>10857470</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>10710067</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>10733303</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>10978777</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <v>10951207</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <v>10995732</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <v>11039247</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="16"/>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
+        <v>11038653</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
-        <v>11010570</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
-        <v>11011839</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>10981895</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>11009444</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>10857617</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
-        <v>10956804</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>10956802</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>10982995</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>10978777</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D45" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>10951207</v>
+        <v>10982246</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>10956804</v>
+        <v>11017183</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>10981895</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>10732806</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
+        <v>10857617</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
+        <v>10956804</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>10956802</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>10982995</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>10956804</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>10732806</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>10719864</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>86</v>
+      <c r="B55" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1630,415 +1705,415 @@
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>40</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>41</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>45</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>46</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>47</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>48</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>49</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>50</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>51</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>52</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>53</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>54</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>55</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>56</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>57</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>58</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>59</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>60</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>61</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>62</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>63</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>64</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>65</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>66</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>67</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>68</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>69</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>70</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>71</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>72</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" t="s">
         <v>76</v>
       </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" t="s">
-        <v>28</v>
-      </c>
-      <c r="V2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>77</v>
       </c>
-      <c r="AA2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT2" t="s">
         <v>78</v>
       </c>
-      <c r="AK2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA2" t="s">
         <v>79</v>
       </c>
-      <c r="AU2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BK2" t="s">
         <v>80</v>
       </c>
-      <c r="BB2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>69</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>81</v>
-      </c>
       <c r="BL2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BM2" t="s">
         <v>71</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>72</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="str">
         <f>IF(A4=B4,"=","!=")</f>
@@ -2047,10 +2122,10 @@
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ref="C5:C68" si="0">IF(A5=B5,"=","!=")</f>
@@ -2059,10 +2134,10 @@
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2071,10 +2146,10 @@
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -2083,10 +2158,10 @@
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2095,10 +2170,10 @@
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2107,10 +2182,10 @@
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2119,10 +2194,10 @@
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2131,10 +2206,10 @@
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2143,10 +2218,10 @@
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -2155,10 +2230,10 @@
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2167,10 +2242,10 @@
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -2179,10 +2254,10 @@
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2191,10 +2266,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2203,10 +2278,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2215,10 +2290,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2227,10 +2302,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -2239,10 +2314,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2251,10 +2326,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -2263,10 +2338,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2275,10 +2350,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -2287,10 +2362,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2299,10 +2374,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -2311,10 +2386,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -2323,10 +2398,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -2335,10 +2410,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -2347,10 +2422,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -2359,10 +2434,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -2371,10 +2446,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -2383,10 +2458,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -2395,10 +2470,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -2407,10 +2482,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -2419,10 +2494,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -2431,10 +2506,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -2443,10 +2518,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -2455,10 +2530,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" t="str">
         <f>IF(A39=B39,"=","!=")</f>
@@ -2467,10 +2542,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -2479,10 +2554,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -2491,10 +2566,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -2503,10 +2578,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -2515,10 +2590,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -2527,10 +2602,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -2539,10 +2614,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -2551,10 +2626,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -2563,10 +2638,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -2575,10 +2650,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -2587,10 +2662,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -2599,10 +2674,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -2611,10 +2686,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -2623,10 +2698,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -2635,10 +2710,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -2647,10 +2722,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -2659,10 +2734,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -2671,10 +2746,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -2683,10 +2758,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -2695,10 +2770,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -2707,10 +2782,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2719,10 +2794,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2731,10 +2806,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2743,10 +2818,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -2755,10 +2830,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -2767,10 +2842,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -2779,10 +2854,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -2791,10 +2866,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="0"/>
@@ -2803,10 +2878,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="0"/>
@@ -2815,10 +2890,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" t="str">
         <f>IF(A69=B69,"=","!=")</f>

</xml_diff>

<commit_message>
Added entry for 11/21
</commit_message>
<xml_diff>
--- a/DailyTicketReport.xlsx
+++ b/DailyTicketReport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="171">
   <si>
     <t>Ticket</t>
   </si>
@@ -280,16 +280,9 @@
   </si>
   <si>
     <t>- No Issue
-- Confirmed some details from the AM.</t>
-  </si>
-  <si>
-    <t>- No Issue
 - Responded to AM's inquiry and proposed a suggestion.</t>
   </si>
   <si>
-    <t>CofPA :I-9 Verifiers not transitioning to the Other Tab form</t>
-  </si>
-  <si>
     <t>- No Issue
 - Startdate was being used only by Completed NewHires Forms export to determine that the user could be exported only after he/she completed the forms not later than 12 days of his/her startdate</t>
   </si>
@@ -301,25 +294,12 @@
 - User's data will be wiped out once 'Custom8' has a value of 'Yes'.This user was imported 2016-07-11. Archived files were not available or deleted later than 20170101 for SUMMA.</t>
   </si>
   <si>
-    <t>Trihealth : query on directory user profile in Case Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CofPA : Request to Toggle on W-2 Election</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
     <t>Conn Appliances Inc. : Increase field length on import package</t>
   </si>
   <si>
-    <t>- No Issue
-- Client wants to be done on UAT</t>
-  </si>
-  <si>
     <t>University of Kentucky :  TS Upgrade: SSIS Analysis</t>
   </si>
   <si>
@@ -330,9 +310,6 @@
 - Development in progress</t>
   </si>
   <si>
-    <t>GDIT : HR404E PDF update Orientation tour v.19 and CSR tour v.16</t>
-  </si>
-  <si>
     <t>PGE : Duplicate Enwisen files on 8/8/17 file</t>
   </si>
   <si>
@@ -354,13 +331,7 @@
 - As per checking, I found that the value for user 08322 on DateofBirth field is '11/25/2022 12:00:00 AM'. No error and warning found in the latest file.</t>
   </si>
   <si>
-    <t>SENA : Suez/Sena Import/Export</t>
-  </si>
-  <si>
     <t>Bechtel : Data not being sent in Data dump files</t>
-  </si>
-  <si>
-    <t>ConAgra : Need notification changed from HRMS to HRDataandAnalysis@conagra.com</t>
   </si>
   <si>
     <t>PNC : New Hire Import Success Notice on hrsdpp02-m</t>
@@ -371,17 +342,8 @@
 Screenshot shows that the file uploaded has 0KB in size.</t>
   </si>
   <si>
-    <t>BectonDickinson :  full time associate does not have access to HR One</t>
-  </si>
-  <si>
-    <t>JPSHealth ~ New hire file</t>
-  </si>
-  <si>
     <t>- No Issue
 - Done as requested</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NavyFederal  : Please reflag users 56502 and 56503</t>
   </si>
   <si>
     <t>NavyFederal  : DMARC implementation requires DNS changes for all OB emails</t>
@@ -430,9 +392,6 @@
 - The date diff makes the ticked not eligible for export, but upon further inspection the 5 give ticket codes were already exported which matches the last edit date.</t>
   </si>
   <si>
-    <t>NavyFederal : Reflag user 51196R01</t>
-  </si>
-  <si>
     <t>- No Issue
 - Files were downloaded from August 1-9</t>
   </si>
@@ -448,9 +407,6 @@
 - User W312057 PoliciesAck reflagged. User will be exported on the next automated export job run.</t>
   </si>
   <si>
-    <t>Bechtel : Language displayed on MyHR Services for an employee on international assignment</t>
-  </si>
-  <si>
     <t>- No Issue
 - This is done as requested to UAT and Prod.</t>
   </si>
@@ -458,24 +414,11 @@
     <t>BannerHealth :  Letters to new hires</t>
   </si>
   <si>
-    <t xml:space="preserve"> Inova Export File Request in UAT</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Informed ICS that files are not existing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BannerHealth  : Full Tour not available to New Hires</t>
-  </si>
-  <si>
     <t>AIR : new hire notification not sent</t>
   </si>
   <si>
     <t>- No Issue
 - Informed AM that there is another file on the path.</t>
-  </si>
-  <si>
-    <t>Bridgestone : UAT manual run</t>
   </si>
   <si>
     <t>- No Issue
@@ -489,9 +432,6 @@
     <t>Benson Fabonan</t>
   </si>
   <si>
-    <t>Nissan : ICS File request</t>
-  </si>
-  <si>
     <t>GDIT : Query on How the "Role2" field is being populated</t>
   </si>
   <si>
@@ -502,18 +442,148 @@
     <t>Bridgestone : Load test file into UAT</t>
   </si>
   <si>
-    <t xml:space="preserve">- No Issue
-- I tried to process the UAT file but I received an error on the email notification. Please check attached file. I will create a test environment to see were it fails on specific parts of the import process but I might take some time. Can we have smaller test user count to test it properly? </t>
+    <t>Inova : Manager did not see manager separtion checklist in their offboarding</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Request logged to deploy changes in PROD. IXS-11040393</t>
+  </si>
+  <si>
+    <t>SENA : Manual off cycle run needed</t>
+  </si>
+  <si>
+    <t>Milliken : Two New Personnel Areas</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Upgrade has no impact aside from SID.</t>
+  </si>
+  <si>
+    <t>CMCD: (KB2 to KB4 Upgrade) SSIS Analysis</t>
+  </si>
+  <si>
+    <t>UMMS: (KB2 to KB4 Upgrade) SSIS Analysis</t>
+  </si>
+  <si>
+    <t>SUMMA : Managers have Enwisen notifications sent to their old emails when hired because e-mails not updated after hire</t>
+  </si>
+  <si>
+    <t>- No Issue
+- File has been successfully loaded to UAT</t>
   </si>
   <si>
     <t>EY : Off-cycle request</t>
   </si>
   <si>
-    <t>Inova : Manager did not see manager separtion checklist in their offboarding</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Request logged to deploy changes in PROD. IXS-11040393</t>
+    <t>- No Issue
+-Successfully loaded the file in UAT.</t>
+  </si>
+  <si>
+    <t>Inova New Hire file structure</t>
+  </si>
+  <si>
+    <t>- No Issue
+-Provided EventTypeCodes and sample users.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Provided the job schedule and files being used.</t>
+  </si>
+  <si>
+    <t>HCA : Missing new hire from flat files</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Provided schedule and files.</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>- No Issue
+- SSIS Imports and Exports do not manage the Reminder notification, it should be via the OB Team</t>
+  </si>
+  <si>
+    <t>Moog: Survey link is not working</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Cannot import file due to live data in the file.</t>
+  </si>
+  <si>
+    <t>Orrick : Manual Run</t>
+  </si>
+  <si>
+    <t>- No Issue
+- No files in inbound folder</t>
+  </si>
+  <si>
+    <t>Sanfrord : Export did not run</t>
+  </si>
+  <si>
+    <t>- No Issue
+-  Will Deploy a fix</t>
+  </si>
+  <si>
+    <t>EY : Import row Failure report on hrsdpp03-m</t>
+  </si>
+  <si>
+    <t>- No Issue
+-  Will deploy changes in production</t>
+  </si>
+  <si>
+    <t>GDIT : PDFS for Kasey O'Neal</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Users have just been exported. Waiting for confirmation to proceed with the reflag.</t>
+  </si>
+  <si>
+    <t>HBC : Default Password</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Explained which export should be checked for the reflagged users.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Promoted to production.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- File was successfully loaded to UAT. Attached success notification email.</t>
+  </si>
+  <si>
+    <t>UMMS PP01 File Transfer</t>
+  </si>
+  <si>
+    <t>Multiple Clientsnot receiving census notifications</t>
+  </si>
+  <si>
+    <t>- No Issue
+-  All indicated clients received a notification as per checking census lod notifications.</t>
+  </si>
+  <si>
+    <t>NorthShore : Elections Mapping</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Requesting to pull the current elections mapping table from NorthShores's Production environment.</t>
+  </si>
+  <si>
+    <t>Bechtel : Missing Column in "Tickets" file - Data dump</t>
+  </si>
+  <si>
+    <t>- No Issue
+- As per checking, the export package can't handle specific dates from previous tickets. This might need time to develop and implement. We may task this out to ICS as this is a new implementation for export process</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Test file loaded in UAT.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- A request has been logged to test the update script in UAT.</t>
   </si>
 </sst>
 </file>
@@ -658,10 +728,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -981,15 +1051,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D55"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.5703125" style="5" customWidth="1"/>
@@ -997,7 +1067,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="1"/>
@@ -1017,417 +1087,435 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>11045499</v>
+      <c r="A3" s="12">
+        <v>11076350</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>11075803</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>11069169</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>11065428</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>11068860</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>11021316</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>10982995</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>11048231</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10981895</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10981491</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10981895</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>10959479</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>10968040</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>11013376</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>10981895</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>10981491</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>10981895</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>10959479</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>10984740</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>11018684</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="16"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>10710067</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>10982909</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>10645887</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>10985054</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>10733303</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="16"/>
-    </row>
-    <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>11053489</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>11076843</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>11013376</v>
+        <v>10855852</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>11033219</v>
+        <v>11028481</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>10986362</v>
+        <v>11013376</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
+        <v>11033219</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>10986362</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>10942832</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>10982995</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>11015181</v>
-      </c>
       <c r="B26" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
+        <v>10982995</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>11015181</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>11002328</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="B29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>11002597</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>11002597</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>10919383</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="B31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>10982995</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="B32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>10912397</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>10978677</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>10916620</v>
-      </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
+        <v>10978677</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>10857470</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>10710067</v>
-      </c>
       <c r="B35" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
@@ -1436,11 +1524,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7"/>
+    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>10710067</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
@@ -1449,118 +1545,120 @@
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="14"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B40" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
-        <v>11009444</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="16"/>
-    </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
-        <v>10978777</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="16"/>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
-        <v>10951207</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="16"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
-        <v>10995732</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="16"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
-        <v>11039247</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="16"/>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
-        <v>11038653</v>
+      <c r="A41" s="2">
+        <v>10719864</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>11066078</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>11065930</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>11059878</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>11055145</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>10982246</v>
+        <v>11050260</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>11017183</v>
+        <v>11047124</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>136</v>
@@ -1569,118 +1667,146 @@
         <v>4</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
+        <v>11047048</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="18">
+        <v>11038653</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>10982246</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>10981895</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>10857617</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
-        <v>10956804</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>10956802</v>
-      </c>
       <c r="B51" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>10982995</v>
+        <v>10857617</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>117</v>
+      <c r="D52" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="16">
         <v>10956804</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>10732806</v>
+        <v>10956802</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>10719864</v>
+        <v>10982995</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D55" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>10956804</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>10732806</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Entry for 11/29
</commit_message>
<xml_diff>
--- a/DailyTicketReport.xlsx
+++ b/DailyTicketReport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="168">
   <si>
     <t>Ticket</t>
   </si>
@@ -270,9 +270,6 @@
     <t>OnboardingID</t>
   </si>
   <si>
-    <t>AIR : rehire was not assigned Tour 1</t>
-  </si>
-  <si>
     <t>TriHealth : JobDesc Import Success Notice</t>
   </si>
   <si>
@@ -283,17 +280,9 @@
 - Responded to AM's inquiry and proposed a suggestion.</t>
   </si>
   <si>
-    <t>- No Issue
-- Startdate was being used only by Completed NewHires Forms export to determine that the user could be exported only after he/she completed the forms not later than 12 days of his/her startdate</t>
-  </si>
-  <si>
     <t>Summa  : Rehires have onboarding records sent twice resulting in tour being wiped out, restarted</t>
   </si>
   <si>
-    <t>- No Issue
-- User's data will be wiped out once 'Custom8' has a value of 'Yes'.This user was imported 2016-07-11. Archived files were not available or deleted later than 20170101 for SUMMA.</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -318,10 +307,6 @@
   </si>
   <si>
     <t>MoheganSun : Missing an Employee</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Error log was set also to 5 days. Please let me know if the client wants to change its value so that we may check longer days of error logs in the future.</t>
   </si>
   <si>
     <t>PGE :  Unable to update Date of Birth for New Hire, Alejandro Ruiz, 08184</t>
@@ -407,22 +392,11 @@
 - User W312057 PoliciesAck reflagged. User will be exported on the next automated export job run.</t>
   </si>
   <si>
-    <t>- No Issue
-- This is done as requested to UAT and Prod.</t>
-  </si>
-  <si>
-    <t>BannerHealth :  Letters to new hires</t>
-  </si>
-  <si>
     <t>AIR : new hire notification not sent</t>
   </si>
   <si>
     <t>- No Issue
 - Informed AM that there is another file on the path.</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Done in UAT</t>
   </si>
   <si>
     <t xml:space="preserve">- No Issue
@@ -475,10 +449,6 @@
     <t>EY : Off-cycle request</t>
   </si>
   <si>
-    <t>- No Issue
--Successfully loaded the file in UAT.</t>
-  </si>
-  <si>
     <t>Inova New Hire file structure</t>
   </si>
   <si>
@@ -490,9 +460,6 @@
 - Provided the job schedule and files being used.</t>
   </si>
   <si>
-    <t>HCA : Missing new hire from flat files</t>
-  </si>
-  <si>
     <t>- No Issue
 - Provided schedule and files.</t>
   </si>
@@ -508,45 +475,6 @@
   </si>
   <si>
     <t>- No Issue
-- Cannot import file due to live data in the file.</t>
-  </si>
-  <si>
-    <t>Orrick : Manual Run</t>
-  </si>
-  <si>
-    <t>- No Issue
-- No files in inbound folder</t>
-  </si>
-  <si>
-    <t>Sanfrord : Export did not run</t>
-  </si>
-  <si>
-    <t>- No Issue
--  Will Deploy a fix</t>
-  </si>
-  <si>
-    <t>EY : Import row Failure report on hrsdpp03-m</t>
-  </si>
-  <si>
-    <t>- No Issue
--  Will deploy changes in production</t>
-  </si>
-  <si>
-    <t>GDIT : PDFS for Kasey O'Neal</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Users have just been exported. Waiting for confirmation to proceed with the reflag.</t>
-  </si>
-  <si>
-    <t>HBC : Default Password</t>
-  </si>
-  <si>
-    <t>- No Issue
-- Explained which export should be checked for the reflagged users.</t>
-  </si>
-  <si>
-    <t>- No Issue
 - Promoted to production.</t>
   </si>
   <si>
@@ -554,16 +482,6 @@
 - File was successfully loaded to UAT. Attached success notification email.</t>
   </si>
   <si>
-    <t>UMMS PP01 File Transfer</t>
-  </si>
-  <si>
-    <t>Multiple Clientsnot receiving census notifications</t>
-  </si>
-  <si>
-    <t>- No Issue
--  All indicated clients received a notification as per checking census lod notifications.</t>
-  </si>
-  <si>
     <t>NorthShore : Elections Mapping</t>
   </si>
   <si>
@@ -582,8 +500,81 @@
 - Test file loaded in UAT.</t>
   </si>
   <si>
-    <t>- No Issue
-- A request has been logged to test the update script in UAT.</t>
+    <t>GeneralDynamics : missing PDFs for Ramon Johnson</t>
+  </si>
+  <si>
+    <t>- No Issue
+- As per checking, this user's PDF was still available on the FTP folder. It was recently exported today. KIndly check attached file for files found on FTP folder</t>
+  </si>
+  <si>
+    <t>- No Issue
+-Test users have not completed any forms yet.</t>
+  </si>
+  <si>
+    <t>NavyFederal : Please reflag user 57082</t>
+  </si>
+  <si>
+    <t>- No Issue
+- IXS# 11087761 was created for deployment. I will update this ticket once it was deployed.</t>
+  </si>
+  <si>
+    <t>AIR : Update Email Template</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Deployed to UAT. Requested test new hire file for testing.</t>
+  </si>
+  <si>
+    <t>JohnsHopkins  : Remove e-mail</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Changes are now in PROD.</t>
+  </si>
+  <si>
+    <t>Sanford: import export issues 11/15-11-26</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Profided RCA from DBA team</t>
+  </si>
+  <si>
+    <t>Conn’s
+Bon Secours (BSHSI)
+CoBank
+Ernst and Young
+Banner Health : import export issues 11/15-11-26</t>
+  </si>
+  <si>
+    <t>Kelloggs : UAT manual run</t>
+  </si>
+  <si>
+    <t>- No Issue
+- Cannot run the file as it is live data.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- File processed</t>
+  </si>
+  <si>
+    <t>- No Issue
+- File ran</t>
+  </si>
+  <si>
+    <t>Concordia : Run census offcycle</t>
+  </si>
+  <si>
+    <t>Arcelor Mittal : TS Upgrade: SSIS Analysis</t>
+  </si>
+  <si>
+    <t>TriHealth  : Please Add Dave Anderson to the TriHealth JobDesc Import Success Notice Email</t>
+  </si>
+  <si>
+    <t>StateofUtah : New hires did not load in manage new hires.</t>
+  </si>
+  <si>
+    <t>- No Issue
+- These users were sent through the UtahHumanResources_newhire_20171127.csv.pgp file but it failed during import. This might be caused by the issue we had with duplicate jobs running. Asked AM to resend the employees.</t>
   </si>
 </sst>
 </file>
@@ -683,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -736,6 +727,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1061,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="1"/>
@@ -1086,72 +1080,74 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>11076350</v>
-      </c>
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>11094827</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>11075803</v>
+        <v>11094191</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>164</v>
+      <c r="D4" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>11069169</v>
+        <v>11094268</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>11065428</v>
+        <v>11090836</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>11068860</v>
+        <v>11090690</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1159,13 +1155,13 @@
         <v>11021316</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1173,13 +1169,13 @@
         <v>10982995</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1187,13 +1183,13 @@
         <v>11048231</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1201,13 +1197,13 @@
         <v>10981895</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1215,41 +1211,41 @@
         <v>10981491</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10981895</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10959479</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,477 +1282,467 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>11053489</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>11076843</v>
-      </c>
-      <c r="B20" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>10886657</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>10919072</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>10855852</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="C20" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>10978677</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="19"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>11028481</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>11013376</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>10857470</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>10982995</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>11033219</v>
+        <v>11087435</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>10986362</v>
+        <v>11082656</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>10942832</v>
+        <v>11053489</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10982995</v>
+        <v>11076843</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>11015181</v>
+        <v>10855852</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
+        <v>11028481</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>11013376</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>11033219</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>10986362</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>11015181</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>11002328</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="B34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>11002597</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="B35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>10919383</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="B36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>10982995</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="B37" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>10912397</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>10978677</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>10857470</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>10710067</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="14"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B42" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>10719864</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>11066078</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>11065930</v>
+        <v>11090330</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D43" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>11059878</v>
+        <v>11080463</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D44" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>11055145</v>
+        <v>11083831</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>140</v>
+      <c r="D45" s="9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>11050260</v>
+        <v>10719864</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>142</v>
+      <c r="D46" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
+        <v>11055145</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>11050260</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>11047124</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B49" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>11047048</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="18">
-        <v>11038653</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
+        <v>11047048</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="18">
+        <v>11038653</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>10982246</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="B52" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>10981895</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="B53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>10857617</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
-        <v>10956804</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>10956802</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>90</v>
@@ -1765,49 +1751,77 @@
         <v>4</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="16">
+        <v>10956804</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>10956802</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>10982995</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="B57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>10956804</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+    </row>
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>10732806</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>84</v>
+      <c r="B59" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>